<commit_message>
[database] edit penerima pengadaan
</commit_message>
<xml_diff>
--- a/templates/HPS Barang.xlsx
+++ b/templates/HPS Barang.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4020" yWindow="735" windowWidth="15480" windowHeight="9210"/>
+    <workbookView xWindow="-4020" yWindow="735" windowWidth="12240" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="BoQ" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">ANALISA!$A$1:$H$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BoQ!$A$1:$G$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BoQ!$A$1:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="144525" iterate="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>No.</t>
   </si>
@@ -61,12 +61,6 @@
     <t>PPn 10%</t>
   </si>
   <si>
-    <t>Sewa/bulan :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dibulatkan : </t>
-  </si>
-  <si>
     <t>$ = 9.143</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
   </si>
   <si>
     <t>GRAND TOTAL / SEWA BULAN</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>#namakadiv#</t>
@@ -209,11 +200,14 @@
   <si>
     <t>#listpanitia#</t>
   </si>
+  <si>
+    <t>TOTAL+PPN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -870,21 +864,49 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
@@ -897,27 +919,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -933,13 +934,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,7 +1023,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1064,7 +1057,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1240,14 +1232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="60" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="60" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1262,42 +1254,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
+      <c r="A2" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
+      <c r="A3" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="1"/>
       <c r="G4" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="15.75" thickBot="1">
@@ -1349,91 +1341,91 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="94"/>
+      <c r="A7" s="91"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="94"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="86"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="95"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="94"/>
+      <c r="A8" s="91"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="94"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="86"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="95"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="94"/>
+      <c r="A9" s="91"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="94"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="86"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="95"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="94"/>
+      <c r="A10" s="91"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="94"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="86"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="95"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="94"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="94"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="86"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="95"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="94"/>
+      <c r="A12" s="91"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="94"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="86"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="95"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="94"/>
+      <c r="A13" s="91"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="94"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="86"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="95"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A14" s="94"/>
+      <c r="A14" s="91"/>
       <c r="B14" s="80"/>
-      <c r="C14" s="94"/>
+      <c r="C14" s="91"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="86"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="95"/>
     </row>
     <row r="15" spans="1:10" ht="1.1499999999999999" customHeight="1" thickBot="1">
-      <c r="A15" s="89"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="97"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="87"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="96"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
       <c r="A16" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="90"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -1449,22 +1441,22 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="63" customHeight="1">
-      <c r="A17" s="88"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="96"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="86"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="95"/>
     </row>
     <row r="18" spans="1:8" ht="2.4500000000000002" customHeight="1" thickBot="1">
-      <c r="A18" s="89"/>
-      <c r="B18" s="91"/>
-      <c r="C18" s="97"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="93"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="87"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="96"/>
     </row>
     <row r="19" spans="1:8" ht="18.600000000000001" customHeight="1">
       <c r="A19" s="2" t="s">
@@ -1486,26 +1478,26 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="54.6" customHeight="1">
-      <c r="A20" s="94"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="94"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="86"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="95"/>
     </row>
     <row r="21" spans="1:8" ht="3" customHeight="1" thickBot="1">
-      <c r="A21" s="95"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="95"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="87"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="96"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="E22" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1519,100 +1511,120 @@
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="E24" s="13" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="E25" s="15" t="s">
+    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="E25" s="13"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="E26" s="15"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="F27" s="15"/>
+      <c r="G27" s="19"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="103" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="103"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="87"/>
+      <c r="F30" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="78"/>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="F26" s="15"/>
-      <c r="G26" s="19"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="93"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="108"/>
-      <c r="F29" s="17" t="s">
+    </row>
+    <row r="31" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A31" s="84"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="87"/>
+      <c r="F31" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A32" s="76"/>
+      <c r="B32" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A30" s="84"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="108"/>
-      <c r="F30" s="17" t="s">
+      <c r="C32" s="76"/>
+      <c r="D32" s="87"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+    </row>
+    <row r="33" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A33" s="98" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A31" s="76"/>
-      <c r="B31" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="108"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-    </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A32" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="85"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="108"/>
-      <c r="F32" s="107" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A33" s="85"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="108"/>
-    </row>
-    <row r="34" spans="1:4" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A34" s="106"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="108"/>
-    </row>
-    <row r="35" spans="1:4" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A35" s="106"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="87"/>
+      <c r="F33" s="86" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A34" s="98"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="87"/>
+    </row>
+    <row r="35" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A35" s="85"/>
       <c r="B35" s="17"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="108"/>
-    </row>
-    <row r="36" spans="1:4" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A36" s="106"/>
-      <c r="B36" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="106"/>
-      <c r="D36" s="108"/>
-    </row>
-    <row r="37" spans="1:4" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A37" s="108"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="108"/>
-      <c r="D37" s="108"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="B38" s="18"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="87"/>
+    </row>
+    <row r="36" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A36" s="85"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="87"/>
+    </row>
+    <row r="37" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A37" s="85"/>
+      <c r="B37" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="85"/>
+      <c r="D37" s="87"/>
+    </row>
+    <row r="38" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A38" s="87"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A33:C34"/>
+    <mergeCell ref="G7:G15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
@@ -1620,23 +1632,6 @@
     <mergeCell ref="C7:C15"/>
     <mergeCell ref="E7:E15"/>
     <mergeCell ref="F7:F15"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A32:C33"/>
-    <mergeCell ref="G7:G15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1645,7 +1640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1676,7 +1671,7 @@
     <row r="1" spans="1:14" ht="18">
       <c r="B1" s="20"/>
       <c r="C1" s="21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1703,14 +1698,14 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:14" s="9" customFormat="1">
-      <c r="A4" s="102" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="104"/>
+      <c r="A4" s="105" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="83"/>
       <c r="G4" s="83"/>
@@ -1719,14 +1714,14 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="29"/>
       <c r="F5" s="30"/>
@@ -1764,7 +1759,7 @@
       <c r="B8" s="37"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="41"/>
       <c r="F8" s="42">
@@ -1788,7 +1783,7 @@
         <v>0.3</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="41"/>
       <c r="F9" s="46">
@@ -1812,7 +1807,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="41"/>
       <c r="F10" s="41">
@@ -1836,7 +1831,7 @@
         <v>0.18</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" s="41"/>
       <c r="F11" s="46">
@@ -1866,29 +1861,29 @@
     </row>
     <row r="13" spans="1:14" s="44" customFormat="1" ht="12.75">
       <c r="A13" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="D13" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="105" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="105" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="101">
+      <c r="E13" s="108" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="104">
         <f>(F8*(1-F9/(1+F11/12)^(F10+1))*(F11/12*(1+F11/12)^F10))/((1+F11/12)^F10-1)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="104">
         <f>(G8*(1-G9/(1+G11/12)^(G10+1))*(G11/12*(1+G11/12)^G10))/((1+G11/12)^G10-1)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="101">
+      <c r="H13" s="104">
         <f>(H8*(1-H9/(1+H11/12)^(H10+1))*(H11/12*(1+H11/12)^H10))/((1+H11/12)^H10-1)</f>
         <v>0</v>
       </c>
@@ -1897,16 +1892,16 @@
     <row r="14" spans="1:14" s="44" customFormat="1" ht="12.75">
       <c r="A14" s="40"/>
       <c r="B14" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="105"/>
+        <v>30</v>
+      </c>
+      <c r="C14" s="108"/>
       <c r="D14" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="105"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
+        <v>31</v>
+      </c>
+      <c r="E14" s="108"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
       <c r="N14" s="45"/>
     </row>
     <row r="15" spans="1:14" s="20" customFormat="1">
@@ -1926,24 +1921,24 @@
     </row>
     <row r="16" spans="1:14" s="20" customFormat="1" ht="16.5">
       <c r="A16" s="52" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="36"/>
       <c r="F16" s="55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G16" s="55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I16" s="51"/>
       <c r="J16" s="50"/>
@@ -1954,7 +1949,7 @@
     <row r="17" spans="1:14" s="20" customFormat="1">
       <c r="A17" s="48"/>
       <c r="B17" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="48"/>
       <c r="D17" s="56">
@@ -1983,7 +1978,7 @@
     <row r="18" spans="1:14" s="20" customFormat="1">
       <c r="A18" s="41"/>
       <c r="B18" s="58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="56">
@@ -2011,7 +2006,7 @@
     <row r="19" spans="1:14" s="20" customFormat="1" ht="16.5">
       <c r="A19" s="41"/>
       <c r="B19" s="58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="56">
@@ -2064,7 +2059,7 @@
       <c r="A21" s="48"/>
       <c r="B21" s="36"/>
       <c r="C21" s="47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
@@ -2089,7 +2084,7 @@
     <row r="22" spans="1:14" s="43" customFormat="1" hidden="1">
       <c r="A22" s="37"/>
       <c r="B22" s="37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="63">
         <v>0</v>
@@ -2143,7 +2138,7 @@
       <c r="B24" s="48"/>
       <c r="C24" s="38"/>
       <c r="D24" s="65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="65"/>
       <c r="F24" s="67">
@@ -2167,7 +2162,7 @@
     <row r="25" spans="1:14" s="20" customFormat="1" hidden="1">
       <c r="A25" s="48"/>
       <c r="B25" s="37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="46">
         <v>0.1</v>
@@ -2197,10 +2192,10 @@
       <c r="B26" s="48"/>
       <c r="C26" s="38"/>
       <c r="D26" s="41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F26" s="69">
         <f>SUM(F24:F25)</f>
@@ -2265,12 +2260,12 @@
     </row>
     <row r="30" spans="1:14">
       <c r="E30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="D32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F32" s="77">
         <f>F30*F24</f>
@@ -2287,7 +2282,7 @@
     </row>
     <row r="33" spans="4:8">
       <c r="D33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F33" s="77">
         <f>F32*0.1</f>
@@ -2304,7 +2299,7 @@
     </row>
     <row r="34" spans="4:8">
       <c r="D34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F34" s="77">
         <f>F33+F32</f>
@@ -2321,7 +2316,7 @@
     </row>
     <row r="36" spans="4:8">
       <c r="D36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F36" s="77">
         <f>F34+G34+H34</f>
@@ -2343,7 +2338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
benerin dokumen pasca kualifikasi pemilihan langsung hingga undangan aanwijzing kecuali rks
</commit_message>
<xml_diff>
--- a/templates/HPS Barang.xlsx
+++ b/templates/HPS Barang.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-4020" yWindow="735" windowWidth="12240" windowHeight="9210"/>
@@ -9,18 +9,17 @@
   <sheets>
     <sheet name="BoQ" sheetId="1" r:id="rId1"/>
     <sheet name="ANALISA" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">ANALISA!$A$1:$H$36</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BoQ!$A$1:$G$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BoQ!$A$1:$G$56</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>No.</t>
   </si>
@@ -64,18 +63,12 @@
     <t>$ = 9.143</t>
   </si>
   <si>
-    <t>PANITIA – B PENGADAAN BARANG / JASA</t>
-  </si>
-  <si>
     <t>PT PLN (PERSERO) KANTOR PUSAT</t>
   </si>
   <si>
     <t>Mengesahkan,</t>
   </si>
   <si>
-    <t>KEPALA DIVISI UMUM DAN MANAJEMEN KANTOR PUSAT</t>
-  </si>
-  <si>
     <t xml:space="preserve">PENYEWA </t>
   </si>
   <si>
@@ -172,36 +165,28 @@
     <t>GRAND TOTAL / SEWA BULAN</t>
   </si>
   <si>
-    <t>#namakadiv#</t>
-  </si>
-  <si>
     <t xml:space="preserve">         RUMUS PERHITUNGAN HARGA SEWA BARANG</t>
   </si>
   <si>
     <t>#namapengadaan#</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Jakarta, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">#tgllengkap# </t>
-    </r>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>#listpanitia#</t>
-  </si>
-  <si>
     <t>TOTAL+PPN</t>
+  </si>
+  <si>
+    <t>#pengesah#</t>
+  </si>
+  <si>
+    <t>#namapengesah#</t>
+  </si>
+  <si>
+    <t>#namapanitia# PENGADAAN BARANG / JASA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakarta, #tgllengkap# </t>
   </si>
 </sst>
 </file>
@@ -684,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -871,26 +856,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -898,26 +892,26 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1236,10 +1230,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1254,37 +1248,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="89" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
+      <c r="A2" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="90" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
+      <c r="A3" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="1"/>
@@ -1341,91 +1335,91 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="91"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="91"/>
+      <c r="C7" s="89"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="95"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="98"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="91"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="91"/>
+      <c r="C8" s="89"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="95"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="98"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="91"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="91"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="95"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="98"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="91"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="91"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="95"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="98"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="91"/>
+      <c r="A11" s="89"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="91"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="91"/>
-      <c r="G11" s="95"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="98"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="91"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="91"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="95"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="98"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="91"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="91"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="95"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="98"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A14" s="91"/>
+      <c r="A14" s="89"/>
       <c r="B14" s="80"/>
-      <c r="C14" s="91"/>
+      <c r="C14" s="89"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="95"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="98"/>
     </row>
     <row r="15" spans="1:10" ht="1.1499999999999999" customHeight="1" thickBot="1">
-      <c r="A15" s="92"/>
-      <c r="B15" s="102"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="96"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="99"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
       <c r="A16" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="101"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -1441,22 +1435,22 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="63" customHeight="1">
-      <c r="A17" s="99"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="97"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="106"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="95"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="98"/>
     </row>
     <row r="18" spans="1:8" ht="2.4500000000000002" customHeight="1" thickBot="1">
-      <c r="A18" s="92"/>
-      <c r="B18" s="101"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="96"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="99"/>
     </row>
     <row r="19" spans="1:8" ht="18.600000000000001" customHeight="1">
       <c r="A19" s="2" t="s">
@@ -1478,26 +1472,26 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="54.6" customHeight="1">
-      <c r="A20" s="91"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="89"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="89"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="95"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="98"/>
     </row>
     <row r="21" spans="1:8" ht="3" customHeight="1" thickBot="1">
-      <c r="A21" s="94"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="94"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="96"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="99"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="E22" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1511,7 +1505,7 @@
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="E24" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1531,14 +1525,14 @@
       <c r="G27" s="19"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="103"/>
-      <c r="C30" s="103"/>
+      <c r="A30" s="104" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="105"/>
+      <c r="C30" s="105"/>
       <c r="D30" s="87"/>
-      <c r="F30" s="17" t="s">
-        <v>14</v>
+      <c r="F30" s="88" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.45" customHeight="1">
@@ -1547,64 +1541,143 @@
       <c r="C31" s="84"/>
       <c r="D31" s="87"/>
       <c r="F31" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="9" customFormat="1" ht="31.15" customHeight="1">
       <c r="A32" s="76"/>
       <c r="B32" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="76"/>
       <c r="D32" s="87"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-    </row>
-    <row r="33" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A33" s="98" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="98"/>
-      <c r="C33" s="98"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+    </row>
+    <row r="33" spans="1:7" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A33" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
       <c r="D33" s="87"/>
-      <c r="F33" s="86" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
-      <c r="A34" s="98"/>
-      <c r="B34" s="98"/>
-      <c r="C34" s="98"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="85"/>
+    </row>
+    <row r="34" spans="1:7" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="A34" s="97"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="97"/>
       <c r="D34" s="87"/>
-    </row>
-    <row r="35" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+    </row>
+    <row r="35" spans="1:7" s="9" customFormat="1" ht="31.15" customHeight="1">
       <c r="A35" s="85"/>
       <c r="B35" s="17"/>
       <c r="C35" s="85"/>
       <c r="D35" s="87"/>
-    </row>
-    <row r="36" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+    </row>
+    <row r="36" spans="1:7" s="9" customFormat="1" ht="29.25" customHeight="1">
       <c r="A36" s="85"/>
       <c r="B36" s="17"/>
       <c r="C36" s="85"/>
       <c r="D36" s="87"/>
-    </row>
-    <row r="37" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+    </row>
+    <row r="37" spans="1:7" s="9" customFormat="1" ht="29.25" customHeight="1">
       <c r="A37" s="85"/>
       <c r="B37" s="82" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C37" s="85"/>
       <c r="D37" s="87"/>
-    </row>
-    <row r="38" spans="1:6" s="9" customFormat="1" ht="31.15" customHeight="1">
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+    </row>
+    <row r="38" spans="1:7" s="9" customFormat="1" ht="29.25" customHeight="1">
       <c r="A38" s="87"/>
       <c r="B38" s="87"/>
       <c r="C38" s="87"/>
       <c r="D38" s="87"/>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+    </row>
+    <row r="39" spans="1:7" ht="29.25" customHeight="1">
       <c r="B39" s="18"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+    </row>
+    <row r="40" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+    </row>
+    <row r="41" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+    </row>
+    <row r="42" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+    </row>
+    <row r="43" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+    </row>
+    <row r="44" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+    </row>
+    <row r="45" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+    </row>
+    <row r="46" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+    </row>
+    <row r="47" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+    </row>
+    <row r="48" spans="1:7" ht="29.25" customHeight="1">
+      <c r="F48" s="76"/>
+      <c r="G48" s="76"/>
+    </row>
+    <row r="49" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+    </row>
+    <row r="50" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+    </row>
+    <row r="51" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+    </row>
+    <row r="52" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+    </row>
+    <row r="53" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+    </row>
+    <row r="54" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+    </row>
+    <row r="55" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+    </row>
+    <row r="56" spans="6:7" ht="29.25" customHeight="1">
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -1635,7 +1708,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="60" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1646,7 +1719,7 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1671,7 +1744,7 @@
     <row r="1" spans="1:14" ht="18">
       <c r="B1" s="20"/>
       <c r="C1" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1698,14 +1771,14 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:14" s="9" customFormat="1">
-      <c r="A4" s="105" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="107"/>
+      <c r="A4" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="110"/>
       <c r="E4" s="26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="83"/>
       <c r="G4" s="83"/>
@@ -1714,14 +1787,14 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="29"/>
       <c r="F5" s="30"/>
@@ -1759,7 +1832,7 @@
       <c r="B8" s="37"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="41"/>
       <c r="F8" s="42">
@@ -1783,7 +1856,7 @@
         <v>0.3</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="41"/>
       <c r="F9" s="46">
@@ -1807,7 +1880,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="41"/>
       <c r="F10" s="41">
@@ -1831,7 +1904,7 @@
         <v>0.18</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="41"/>
       <c r="F11" s="46">
@@ -1861,29 +1934,29 @@
     </row>
     <row r="13" spans="1:14" s="44" customFormat="1" ht="12.75">
       <c r="A13" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="D13" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="108" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="108" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="104">
+      <c r="E13" s="111" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="107">
         <f>(F8*(1-F9/(1+F11/12)^(F10+1))*(F11/12*(1+F11/12)^F10))/((1+F11/12)^F10-1)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="104">
+      <c r="G13" s="107">
         <f>(G8*(1-G9/(1+G11/12)^(G10+1))*(G11/12*(1+G11/12)^G10))/((1+G11/12)^G10-1)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="104">
+      <c r="H13" s="107">
         <f>(H8*(1-H9/(1+H11/12)^(H10+1))*(H11/12*(1+H11/12)^H10))/((1+H11/12)^H10-1)</f>
         <v>0</v>
       </c>
@@ -1892,16 +1965,16 @@
     <row r="14" spans="1:14" s="44" customFormat="1" ht="12.75">
       <c r="A14" s="40"/>
       <c r="B14" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="108"/>
+        <v>28</v>
+      </c>
+      <c r="C14" s="111"/>
       <c r="D14" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
+        <v>29</v>
+      </c>
+      <c r="E14" s="111"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
       <c r="N14" s="45"/>
     </row>
     <row r="15" spans="1:14" s="20" customFormat="1">
@@ -1921,24 +1994,24 @@
     </row>
     <row r="16" spans="1:14" s="20" customFormat="1" ht="16.5">
       <c r="A16" s="52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="54" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="36"/>
       <c r="F16" s="55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G16" s="55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I16" s="51"/>
       <c r="J16" s="50"/>
@@ -1949,7 +2022,7 @@
     <row r="17" spans="1:14" s="20" customFormat="1">
       <c r="A17" s="48"/>
       <c r="B17" s="36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="48"/>
       <c r="D17" s="56">
@@ -1978,7 +2051,7 @@
     <row r="18" spans="1:14" s="20" customFormat="1">
       <c r="A18" s="41"/>
       <c r="B18" s="58" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="56">
@@ -2006,7 +2079,7 @@
     <row r="19" spans="1:14" s="20" customFormat="1" ht="16.5">
       <c r="A19" s="41"/>
       <c r="B19" s="58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="56">
@@ -2059,7 +2132,7 @@
       <c r="A21" s="48"/>
       <c r="B21" s="36"/>
       <c r="C21" s="47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
@@ -2084,7 +2157,7 @@
     <row r="22" spans="1:14" s="43" customFormat="1" hidden="1">
       <c r="A22" s="37"/>
       <c r="B22" s="37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="63">
         <v>0</v>
@@ -2138,7 +2211,7 @@
       <c r="B24" s="48"/>
       <c r="C24" s="38"/>
       <c r="D24" s="65" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" s="65"/>
       <c r="F24" s="67">
@@ -2162,7 +2235,7 @@
     <row r="25" spans="1:14" s="20" customFormat="1" hidden="1">
       <c r="A25" s="48"/>
       <c r="B25" s="37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="46">
         <v>0.1</v>
@@ -2192,10 +2265,10 @@
       <c r="B26" s="48"/>
       <c r="C26" s="38"/>
       <c r="D26" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F26" s="69">
         <f>SUM(F24:F25)</f>
@@ -2260,12 +2333,12 @@
     </row>
     <row r="30" spans="1:14">
       <c r="E30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="D32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F32" s="77">
         <f>F30*F24</f>
@@ -2282,7 +2355,7 @@
     </row>
     <row r="33" spans="4:8">
       <c r="D33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F33" s="77">
         <f>F32*0.1</f>
@@ -2299,7 +2372,7 @@
     </row>
     <row r="34" spans="4:8">
       <c r="D34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F34" s="77">
         <f>F33+F32</f>
@@ -2316,7 +2389,7 @@
     </row>
     <row r="36" spans="4:8">
       <c r="D36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F36" s="77">
         <f>F34+G34+H34</f>
@@ -2335,16 +2408,4 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>